<commit_message>
replaced append with concat function to stop using old function type
</commit_message>
<xml_diff>
--- a/log/66 HULDE&VO.xlsx
+++ b/log/66 HULDE&VO.xlsx
@@ -16,16 +16,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
+    <t>Mollie-ID</t>
+  </si>
+  <si>
+    <t>ID-nummer</t>
+  </si>
+  <si>
+    <t>Naam</t>
+  </si>
+  <si>
     <t>Aantal</t>
-  </si>
-  <si>
-    <t>ID-nummer</t>
-  </si>
-  <si>
-    <t>Mollie-ID</t>
-  </si>
-  <si>
-    <t>Naam</t>
   </si>
   <si>
     <t>mollie_ABC123</t>
@@ -410,17 +410,17 @@
       </c>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>4</v>
       </c>
       <c r="B2">
         <v>1445758</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" t="s">
         <v>5</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>